<commit_message>
more commercial fishers and fleet xlsx
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb57/raw/Table6.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb57/raw/Table6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb57/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FB5391-87C1-984F-A512-F987A07D0467}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9C7843-F126-8546-AA08-51E52D867960}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Region of home port</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Total check</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
   </si>
 </sst>
 </file>
@@ -86,7 +89,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -178,23 +181,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -513,10 +516,10 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="19"/>
     <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
@@ -525,7 +528,7 @@
     <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="102" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="68" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -567,7 +570,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -586,7 +589,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -609,7 +612,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
@@ -632,7 +635,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
@@ -653,8 +656,10 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="B7" s="11">
         <v>228</v>
       </c>
@@ -697,7 +702,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -741,7 +746,7 @@
         <v>3110</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="16" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -770,13 +775,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
     </row>
   </sheetData>

</xml_diff>